<commit_message>
upload google papago compare
</commit_message>
<xml_diff>
--- a/17_TwigFarm/Gcon_Diff/data_crawling/1_엑셀.xlsx
+++ b/17_TwigFarm/Gcon_Diff/data_crawling/1_엑셀.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jihyeoh/Desktop/Desktop - Jeewon의 iMac/GIT/TIL/17_TwigFarm/Gcon_Diff/data_crawling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6044BD6-A7F2-0A42-8E32-18FD9A4AE92F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1B16FEC-1A9B-8E49-AE7E-6C597D518460}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="24900" yWindow="500" windowWidth="26300" windowHeight="24360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,14 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$171</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$172</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="342">
   <si>
     <t>No</t>
   </si>
@@ -241,9 +241,6 @@
     <t>40</t>
   </si>
   <si>
-    <t xml:space="preserve"> 소리가 날카롭고 커서 듣기에 괴롭다. 너무 여러 번 들어서 듣기가 싫다. </t>
-  </si>
-  <si>
     <t>41</t>
   </si>
   <si>
@@ -1006,9 +1003,6 @@
     <t xml:space="preserve"> 보기에 아니꼬워 비위에 거슬리게 밉다. </t>
   </si>
   <si>
-    <t>구글</t>
-  </si>
-  <si>
     <t xml:space="preserve">무섭거나 놀라서 날카롭게 신경이 곤두서다. </t>
   </si>
   <si>
@@ -1033,97 +1027,28 @@
     <t xml:space="preserve">상대방이 세우는 자존심 또는 기를 꺾다. 자존심을 무너뜨리다. </t>
   </si>
   <si>
-    <t>Be on the brink of hair</t>
-  </si>
-  <si>
-    <t>He was scared or surprised, so he was keenly nervous.</t>
-  </si>
-  <si>
-    <t>The eyebrows are not hard</t>
-  </si>
-  <si>
-    <t>Not surprised and very casual.</t>
-  </si>
-  <si>
-    <t>In the blink of an eye</t>
-  </si>
-  <si>
-    <t>Very short moment</t>
-  </si>
-  <si>
-    <t>meet one's eye</t>
-  </si>
-  <si>
-    <t>Stand out prominently</t>
-  </si>
-  <si>
-    <t>Eye fit</t>
-  </si>
-  <si>
-    <t>The two people's hearts and eyes communicate with each other.</t>
-  </si>
-  <si>
-    <t>High value desiring</t>
-  </si>
-  <si>
-    <t>There is a habit of looking for only good things more than enough.</t>
-  </si>
-  <si>
-    <t>Losing reason by being shocked or obsessed with something.</t>
-  </si>
-  <si>
-    <t>Eyes turn over</t>
-  </si>
-  <si>
-    <t>No one's eyes open</t>
-  </si>
-  <si>
-    <t>Too busy.</t>
-  </si>
-  <si>
-    <t>Break one's nose</t>
-  </si>
-  <si>
-    <t>It breaks the pride or spirit that the other person builds up. Destroy pride</t>
-  </si>
-  <si>
-    <t>Flatten the nose</t>
-  </si>
-  <si>
-    <t>Be terribly embarrassed or depressed.</t>
-  </si>
-  <si>
-    <t>Have a high nose</t>
-  </si>
-  <si>
-    <t>There is a momentum to pretend and show off.</t>
-  </si>
-  <si>
-    <t>Money in the nose</t>
-  </si>
-  <si>
     <t xml:space="preserve">어린아이가 가진 적은 돈. </t>
   </si>
   <si>
-    <t>Little money a child has.</t>
-  </si>
-  <si>
-    <t>Face each other close together</t>
-  </si>
-  <si>
-    <t>Drool in the mouth</t>
-  </si>
-  <si>
-    <t>Nose to nose</t>
-  </si>
-  <si>
-    <t>Saying very nicely about other people or things over and over again.</t>
-  </si>
-  <si>
-    <t>We do not carelessly transfer little words or knowing things.</t>
-  </si>
-  <si>
-    <t>Have a heavy mouth</t>
+    <t xml:space="preserve"> 소리가 날카롭고 커서 듣기에 괴롭다. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">너무 여러 번 들어서 듣기가 싫다. </t>
+  </si>
+  <si>
+    <t>It's uncomfortable to look at, and I hate it.</t>
+  </si>
+  <si>
+    <t>Ugly</t>
+  </si>
+  <si>
+    <t>Uselessly, too much to meddle in anything.</t>
+  </si>
+  <si>
+    <t>The remote area is wide</t>
+  </si>
+  <si>
+    <t>Install it before it even happens.</t>
   </si>
 </sst>
 </file>
@@ -1529,10 +1454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C171"/>
+  <dimension ref="A1:C173"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="192" zoomScaleNormal="192" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" zoomScale="192" zoomScaleNormal="192" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -1547,9 +1472,6 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>327</v>
-      </c>
     </row>
     <row r="2" spans="1:3" ht="35">
       <c r="A2" t="s">
@@ -1558,20 +1480,16 @@
       <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>336</v>
-      </c>
+      <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:3" ht="35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>328</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>337</v>
-      </c>
+        <v>326</v>
+      </c>
+      <c r="C3" s="2"/>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
@@ -1580,19 +1498,13 @@
       <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" t="s">
-        <v>338</v>
-      </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>329</v>
-      </c>
-      <c r="C5" t="s">
-        <v>339</v>
+        <v>327</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -1602,19 +1514,13 @@
       <c r="B6" t="s">
         <v>9</v>
       </c>
-      <c r="C6" t="s">
-        <v>340</v>
-      </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>330</v>
-      </c>
-      <c r="C7" t="s">
-        <v>341</v>
+        <v>328</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="35">
@@ -1624,19 +1530,14 @@
       <c r="B8" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>342</v>
-      </c>
+      <c r="C8" s="2"/>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>331</v>
-      </c>
-      <c r="C9" t="s">
-        <v>343</v>
+        <v>329</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -1646,19 +1547,13 @@
       <c r="B10" t="s">
         <v>15</v>
       </c>
-      <c r="C10" t="s">
-        <v>344</v>
-      </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
         <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>332</v>
-      </c>
-      <c r="C11" t="s">
-        <v>345</v>
+        <v>330</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -1668,9 +1563,6 @@
       <c r="B12" t="s">
         <v>18</v>
       </c>
-      <c r="C12" t="s">
-        <v>346</v>
-      </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
@@ -1679,9 +1571,6 @@
       <c r="B13" t="s">
         <v>20</v>
       </c>
-      <c r="C13" t="s">
-        <v>347</v>
-      </c>
     </row>
     <row r="14" spans="1:3" ht="35">
       <c r="A14" t="s">
@@ -1690,20 +1579,16 @@
       <c r="B14" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>349</v>
-      </c>
+      <c r="C14" s="2"/>
     </row>
     <row r="15" spans="1:3" ht="35">
       <c r="A15" t="s">
         <v>23</v>
       </c>
       <c r="B15" t="s">
-        <v>333</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>348</v>
-      </c>
+        <v>331</v>
+      </c>
+      <c r="C15" s="2"/>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
@@ -1712,19 +1597,13 @@
       <c r="B16" t="s">
         <v>25</v>
       </c>
-      <c r="C16" t="s">
-        <v>350</v>
-      </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
         <v>26</v>
       </c>
       <c r="B17" t="s">
-        <v>334</v>
-      </c>
-      <c r="C17" t="s">
-        <v>351</v>
+        <v>332</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="35">
@@ -1734,20 +1613,16 @@
       <c r="B18" t="s">
         <v>28</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>352</v>
-      </c>
+      <c r="C18" s="2"/>
     </row>
     <row r="19" spans="1:3" ht="17">
       <c r="A19" t="s">
         <v>29</v>
       </c>
       <c r="B19" t="s">
-        <v>335</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>353</v>
-      </c>
+        <v>333</v>
+      </c>
+      <c r="C19" s="3"/>
     </row>
     <row r="20" spans="1:3" ht="35">
       <c r="A20" t="s">
@@ -1756,9 +1631,7 @@
       <c r="B20" t="s">
         <v>31</v>
       </c>
-      <c r="C20" s="2" t="s">
-        <v>354</v>
-      </c>
+      <c r="C20" s="2"/>
     </row>
     <row r="21" spans="1:3" ht="35">
       <c r="A21" t="s">
@@ -1767,9 +1640,7 @@
       <c r="B21" t="s">
         <v>33</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>355</v>
-      </c>
+      <c r="C21" s="2"/>
     </row>
     <row r="22" spans="1:3" ht="35">
       <c r="A22" t="s">
@@ -1778,9 +1649,7 @@
       <c r="B22" t="s">
         <v>35</v>
       </c>
-      <c r="C22" s="2" t="s">
-        <v>356</v>
-      </c>
+      <c r="C22" s="2"/>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
@@ -1789,9 +1658,6 @@
       <c r="B23" t="s">
         <v>37</v>
       </c>
-      <c r="C23" t="s">
-        <v>357</v>
-      </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
@@ -1800,20 +1666,15 @@
       <c r="B24" t="s">
         <v>39</v>
       </c>
-      <c r="C24" t="s">
-        <v>358</v>
-      </c>
     </row>
     <row r="25" spans="1:3" ht="37">
       <c r="A25" t="s">
         <v>40</v>
       </c>
       <c r="B25" t="s">
-        <v>359</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>360</v>
-      </c>
+        <v>334</v>
+      </c>
+      <c r="C25" s="4"/>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
@@ -1822,9 +1683,6 @@
       <c r="B26" t="s">
         <v>42</v>
       </c>
-      <c r="C26" t="s">
-        <v>363</v>
-      </c>
     </row>
     <row r="27" spans="1:3" ht="35">
       <c r="A27" t="s">
@@ -1833,9 +1691,7 @@
       <c r="B27" t="s">
         <v>44</v>
       </c>
-      <c r="C27" s="2" t="s">
-        <v>361</v>
-      </c>
+      <c r="C27" s="2"/>
     </row>
     <row r="28" spans="1:3" ht="35">
       <c r="A28" t="s">
@@ -1844,9 +1700,7 @@
       <c r="B28" t="s">
         <v>46</v>
       </c>
-      <c r="C28" s="2" t="s">
-        <v>362</v>
-      </c>
+      <c r="C28" s="2"/>
     </row>
     <row r="29" spans="1:3" ht="35">
       <c r="A29" t="s">
@@ -1855,9 +1709,7 @@
       <c r="B29" t="s">
         <v>48</v>
       </c>
-      <c r="C29" s="2" t="s">
-        <v>364</v>
-      </c>
+      <c r="C29" s="2"/>
     </row>
     <row r="30" spans="1:3" ht="35">
       <c r="A30" t="s">
@@ -1866,9 +1718,7 @@
       <c r="B30" t="s">
         <v>50</v>
       </c>
-      <c r="C30" s="2" t="s">
-        <v>366</v>
-      </c>
+      <c r="C30" s="2"/>
     </row>
     <row r="31" spans="1:3" ht="35">
       <c r="A31" t="s">
@@ -1877,60 +1727,63 @@
       <c r="B31" t="s">
         <v>52</v>
       </c>
-      <c r="C31" s="2" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="17">
+      <c r="C31" s="2"/>
+    </row>
+    <row r="32" spans="1:3" ht="35">
       <c r="A32" t="s">
         <v>53</v>
       </c>
       <c r="B32" t="s">
         <v>54</v>
       </c>
-      <c r="C32" s="3"/>
-    </row>
-    <row r="33" spans="1:2">
+      <c r="C32" s="2"/>
+    </row>
+    <row r="33" spans="1:3" ht="35">
       <c r="A33" t="s">
         <v>55</v>
       </c>
       <c r="B33" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="34" spans="1:2">
+      <c r="C33" s="2"/>
+    </row>
+    <row r="34" spans="1:3" ht="35">
       <c r="A34" t="s">
         <v>57</v>
       </c>
       <c r="B34" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="35" spans="1:2">
+      <c r="C34" s="2"/>
+    </row>
+    <row r="35" spans="1:3" ht="35">
       <c r="A35" t="s">
         <v>59</v>
       </c>
       <c r="B35" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="36" spans="1:2">
+      <c r="C35" s="2"/>
+    </row>
+    <row r="36" spans="1:3" ht="35">
       <c r="A36" t="s">
         <v>61</v>
       </c>
       <c r="B36" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="37" spans="1:2">
+      <c r="C36" s="2"/>
+    </row>
+    <row r="37" spans="1:3" ht="35">
       <c r="A37" t="s">
         <v>63</v>
       </c>
       <c r="B37" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="38" spans="1:2">
+      <c r="C37" s="2"/>
+    </row>
+    <row r="38" spans="1:3">
       <c r="A38" t="s">
         <v>65</v>
       </c>
@@ -1938,7 +1791,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:3">
       <c r="A39" t="s">
         <v>67</v>
       </c>
@@ -1946,1064 +1799,1109 @@
         <v>68</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:3" ht="35">
       <c r="A40" t="s">
         <v>69</v>
       </c>
       <c r="B40" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="41" spans="1:2">
+      <c r="C40" s="2"/>
+    </row>
+    <row r="41" spans="1:3" ht="35">
       <c r="A41" t="s">
         <v>71</v>
       </c>
       <c r="B41" t="s">
+        <v>335</v>
+      </c>
+      <c r="C41" s="2"/>
+    </row>
+    <row r="42" spans="1:3" ht="35">
+      <c r="A42" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="42" spans="1:2">
-      <c r="A42" t="s">
+      <c r="B42" t="s">
+        <v>336</v>
+      </c>
+      <c r="C42" s="2"/>
+    </row>
+    <row r="43" spans="1:3" ht="35">
+      <c r="A43" t="s">
+        <v>74</v>
+      </c>
+      <c r="B43" t="s">
         <v>73</v>
       </c>
-      <c r="B42" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2">
-      <c r="A43" t="s">
+      <c r="C43" s="2"/>
+    </row>
+    <row r="44" spans="1:3" ht="35">
+      <c r="A44" t="s">
+        <v>76</v>
+      </c>
+      <c r="B44" t="s">
         <v>75</v>
       </c>
-      <c r="B43" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2">
-      <c r="A44" t="s">
+      <c r="C44" s="2"/>
+    </row>
+    <row r="45" spans="1:3" ht="35">
+      <c r="A45" t="s">
+        <v>78</v>
+      </c>
+      <c r="B45" t="s">
         <v>77</v>
       </c>
-      <c r="B44" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2">
-      <c r="A45" t="s">
+      <c r="C45" s="2"/>
+    </row>
+    <row r="46" spans="1:3" ht="35">
+      <c r="A46" t="s">
+        <v>80</v>
+      </c>
+      <c r="B46" t="s">
         <v>79</v>
       </c>
-      <c r="B45" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2">
-      <c r="A46" t="s">
+      <c r="C46" s="2"/>
+    </row>
+    <row r="47" spans="1:3" ht="35">
+      <c r="A47" t="s">
+        <v>82</v>
+      </c>
+      <c r="B47" t="s">
         <v>81</v>
       </c>
-      <c r="B46" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2">
-      <c r="A47" t="s">
+      <c r="C47" s="2"/>
+    </row>
+    <row r="48" spans="1:3" ht="35">
+      <c r="A48" t="s">
+        <v>84</v>
+      </c>
+      <c r="B48" t="s">
         <v>83</v>
       </c>
-      <c r="B47" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2">
-      <c r="A48" t="s">
+      <c r="C48" s="2"/>
+    </row>
+    <row r="49" spans="1:3" ht="35">
+      <c r="A49" t="s">
+        <v>86</v>
+      </c>
+      <c r="B49" t="s">
         <v>85</v>
       </c>
-      <c r="B48" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2">
-      <c r="A49" t="s">
+      <c r="C49" s="2"/>
+    </row>
+    <row r="50" spans="1:3" ht="35">
+      <c r="A50" t="s">
+        <v>88</v>
+      </c>
+      <c r="B50" t="s">
         <v>87</v>
       </c>
-      <c r="B49" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2">
-      <c r="A50" t="s">
+      <c r="C50" s="2"/>
+    </row>
+    <row r="51" spans="1:3" ht="35">
+      <c r="A51" t="s">
+        <v>90</v>
+      </c>
+      <c r="B51" t="s">
         <v>89</v>
       </c>
-      <c r="B50" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2">
-      <c r="A51" t="s">
+      <c r="C51" s="2"/>
+    </row>
+    <row r="52" spans="1:3" ht="35">
+      <c r="A52" t="s">
+        <v>92</v>
+      </c>
+      <c r="B52" t="s">
         <v>91</v>
       </c>
-      <c r="B51" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2">
-      <c r="A52" t="s">
+      <c r="C52" s="2"/>
+    </row>
+    <row r="53" spans="1:3" ht="35">
+      <c r="A53" t="s">
+        <v>94</v>
+      </c>
+      <c r="B53" t="s">
         <v>93</v>
       </c>
-      <c r="B52" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2">
-      <c r="A53" t="s">
+      <c r="C53" s="2"/>
+    </row>
+    <row r="54" spans="1:3" ht="35">
+      <c r="A54" t="s">
+        <v>96</v>
+      </c>
+      <c r="B54" t="s">
         <v>95</v>
       </c>
-      <c r="B53" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2">
-      <c r="A54" t="s">
+      <c r="C54" s="2"/>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" t="s">
+        <v>98</v>
+      </c>
+      <c r="B55" t="s">
         <v>97</v>
       </c>
-      <c r="B54" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2">
-      <c r="A55" t="s">
+    </row>
+    <row r="56" spans="1:3" ht="35">
+      <c r="A56" t="s">
+        <v>100</v>
+      </c>
+      <c r="B56" t="s">
         <v>99</v>
       </c>
-      <c r="B55" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2">
-      <c r="A56" t="s">
+      <c r="C56" s="2"/>
+    </row>
+    <row r="57" spans="1:3" ht="35">
+      <c r="A57" t="s">
+        <v>102</v>
+      </c>
+      <c r="B57" t="s">
         <v>101</v>
       </c>
-      <c r="B56" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2">
-      <c r="A57" t="s">
+      <c r="C57" s="2"/>
+    </row>
+    <row r="58" spans="1:3" ht="35">
+      <c r="A58" t="s">
+        <v>104</v>
+      </c>
+      <c r="B58" t="s">
         <v>103</v>
       </c>
-      <c r="B57" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2">
-      <c r="A58" t="s">
+      <c r="C58" s="2"/>
+    </row>
+    <row r="59" spans="1:3" ht="17">
+      <c r="A59" t="s">
+        <v>106</v>
+      </c>
+      <c r="B59" t="s">
         <v>105</v>
       </c>
-      <c r="B58" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2">
-      <c r="A59" t="s">
+      <c r="C59" s="3"/>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" t="s">
+        <v>108</v>
+      </c>
+      <c r="B60" t="s">
         <v>107</v>
       </c>
-      <c r="B59" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2">
-      <c r="A60" t="s">
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" t="s">
+        <v>110</v>
+      </c>
+      <c r="B61" t="s">
         <v>109</v>
       </c>
-      <c r="B60" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2">
-      <c r="A61" t="s">
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62" t="s">
+        <v>112</v>
+      </c>
+      <c r="B62" t="s">
         <v>111</v>
       </c>
-      <c r="B61" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2">
-      <c r="A62" t="s">
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63" t="s">
+        <v>114</v>
+      </c>
+      <c r="B63" t="s">
         <v>113</v>
       </c>
-      <c r="B62" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2">
-      <c r="A63" t="s">
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64" t="s">
+        <v>116</v>
+      </c>
+      <c r="B64" t="s">
         <v>115</v>
-      </c>
-      <c r="B63" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2">
-      <c r="A64" t="s">
-        <v>117</v>
-      </c>
-      <c r="B64" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B65" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B66" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B67" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="68" spans="1:2">
       <c r="A68" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B68" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="69" spans="1:2">
       <c r="A69" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B69" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="70" spans="1:2">
       <c r="A70" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B70" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="71" spans="1:2">
       <c r="A71" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B71" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="72" spans="1:2">
       <c r="A72" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B72" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="73" spans="1:2">
       <c r="A73" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B73" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="74" spans="1:2">
       <c r="A74" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B74" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="75" spans="1:2">
       <c r="A75" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B75" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="76" spans="1:2">
       <c r="A76" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B76" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="77" spans="1:2">
       <c r="A77" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B77" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="78" spans="1:2">
       <c r="A78" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B78" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="79" spans="1:2">
       <c r="A79" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B79" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="80" spans="1:2">
       <c r="A80" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B80" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="81" spans="1:2">
       <c r="A81" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B81" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="82" spans="1:2">
       <c r="A82" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B82" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="83" spans="1:2">
       <c r="A83" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B83" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="84" spans="1:2">
       <c r="A84" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B84" t="s">
-        <v>141</v>
+        <v>154</v>
       </c>
     </row>
     <row r="85" spans="1:2">
       <c r="A85" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B85" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="86" spans="1:2">
       <c r="A86" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B86" t="s">
-        <v>159</v>
+        <v>142</v>
       </c>
     </row>
     <row r="87" spans="1:2">
       <c r="A87" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B87" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="88" spans="1:2">
       <c r="A88" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B88" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="89" spans="1:2">
       <c r="A89" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B89" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="90" spans="1:2">
       <c r="A90" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B90" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="91" spans="1:2">
       <c r="A91" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B91" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="92" spans="1:2">
       <c r="A92" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B92" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="93" spans="1:2">
       <c r="A93" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B93" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="94" spans="1:2">
       <c r="A94" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B94" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="95" spans="1:2">
       <c r="A95" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B95" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="96" spans="1:2">
       <c r="A96" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B96" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="97" spans="1:2">
       <c r="A97" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B97" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="98" spans="1:2">
       <c r="A98" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B98" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="99" spans="1:2">
       <c r="A99" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B99" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="100" spans="1:2">
       <c r="A100" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B100" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="101" spans="1:2">
       <c r="A101" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B101" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="102" spans="1:2">
       <c r="A102" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B102" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="103" spans="1:2">
       <c r="A103" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B103" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="104" spans="1:2">
       <c r="A104" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B104" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="105" spans="1:2">
       <c r="A105" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B105" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="106" spans="1:2">
       <c r="A106" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B106" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="107" spans="1:2">
       <c r="A107" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B107" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="108" spans="1:2">
       <c r="A108" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B108" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="109" spans="1:2">
       <c r="A109" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B109" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="110" spans="1:2">
       <c r="A110" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B110" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="111" spans="1:2">
       <c r="A111" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B111" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="112" spans="1:2">
       <c r="A112" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B112" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="113" spans="1:2">
       <c r="A113" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B113" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="114" spans="1:2">
       <c r="A114" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B114" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="115" spans="1:2">
       <c r="A115" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B115" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="116" spans="1:2">
       <c r="A116" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B116" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="117" spans="1:2">
       <c r="A117" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B117" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="118" spans="1:2">
       <c r="A118" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B118" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="119" spans="1:2">
       <c r="A119" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B119" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="120" spans="1:2">
       <c r="A120" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B120" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="121" spans="1:2">
       <c r="A121" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B121" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="122" spans="1:2">
       <c r="A122" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B122" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="123" spans="1:2">
       <c r="A123" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B123" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="124" spans="1:2">
       <c r="A124" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B124" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
     </row>
     <row r="125" spans="1:2">
       <c r="A125" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B125" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="126" spans="1:2">
       <c r="A126" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B126" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="127" spans="1:2">
       <c r="A127" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B127" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="128" spans="1:2">
       <c r="A128" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B128" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="129" spans="1:2">
       <c r="A129" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B129" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="130" spans="1:2">
       <c r="A130" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B130" t="s">
-        <v>171</v>
+        <v>244</v>
       </c>
     </row>
     <row r="131" spans="1:2">
       <c r="A131" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B131" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="132" spans="1:2">
       <c r="A132" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B132" t="s">
-        <v>249</v>
+        <v>172</v>
       </c>
     </row>
     <row r="133" spans="1:2">
       <c r="A133" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B133" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="134" spans="1:2">
       <c r="A134" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B134" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="135" spans="1:2">
       <c r="A135" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B135" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="136" spans="1:2">
       <c r="A136" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B136" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="137" spans="1:2">
       <c r="A137" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B137" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="138" spans="1:2">
       <c r="A138" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B138" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
     </row>
     <row r="139" spans="1:2">
       <c r="A139" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B139" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
     </row>
     <row r="140" spans="1:2">
       <c r="A140" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B140" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="141" spans="1:2">
       <c r="A141" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B141" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
     </row>
     <row r="142" spans="1:2">
       <c r="A142" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B142" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="143" spans="1:2">
       <c r="A143" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B143" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="144" spans="1:2">
       <c r="A144" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B144" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
     </row>
     <row r="145" spans="1:2">
       <c r="A145" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B145" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="146" spans="1:2">
       <c r="A146" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B146" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="147" spans="1:2">
       <c r="A147" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B147" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="148" spans="1:2">
       <c r="A148" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B148" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="149" spans="1:2">
       <c r="A149" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B149" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
     <row r="150" spans="1:2">
       <c r="A150" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B150" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="151" spans="1:2">
       <c r="A151" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B151" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="152" spans="1:2">
       <c r="A152" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B152" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
     </row>
     <row r="153" spans="1:2">
       <c r="A153" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B153" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="154" spans="1:2">
       <c r="A154" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B154" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
     </row>
     <row r="155" spans="1:2">
       <c r="A155" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B155" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="156" spans="1:2">
       <c r="A156" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B156" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
     <row r="157" spans="1:2">
       <c r="A157" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B157" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
     </row>
     <row r="158" spans="1:2">
       <c r="A158" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B158" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
     </row>
     <row r="159" spans="1:2">
       <c r="A159" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B159" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
     </row>
     <row r="160" spans="1:2">
       <c r="A160" t="s">
+        <v>303</v>
+      </c>
+      <c r="B160" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3">
+      <c r="A161" t="s">
+        <v>305</v>
+      </c>
+      <c r="B161" t="s">
         <v>304</v>
       </c>
-      <c r="B160" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="161" spans="1:2">
-      <c r="A161" t="s">
+    </row>
+    <row r="162" spans="1:3">
+      <c r="A162" t="s">
+        <v>307</v>
+      </c>
+      <c r="B162" t="s">
         <v>306</v>
       </c>
-      <c r="B161" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="162" spans="1:2">
-      <c r="A162" t="s">
+    </row>
+    <row r="163" spans="1:3">
+      <c r="A163" t="s">
+        <v>309</v>
+      </c>
+      <c r="B163" t="s">
         <v>308</v>
       </c>
-      <c r="B162" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="163" spans="1:2">
-      <c r="A163" t="s">
+    </row>
+    <row r="164" spans="1:3">
+      <c r="A164" t="s">
+        <v>311</v>
+      </c>
+      <c r="B164" t="s">
         <v>310</v>
       </c>
-      <c r="B163" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="164" spans="1:2">
-      <c r="A164" t="s">
+    </row>
+    <row r="165" spans="1:3">
+      <c r="A165" t="s">
+        <v>313</v>
+      </c>
+      <c r="B165" t="s">
         <v>312</v>
       </c>
-      <c r="B164" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="165" spans="1:2">
-      <c r="A165" t="s">
+    </row>
+    <row r="166" spans="1:3">
+      <c r="A166" t="s">
+        <v>315</v>
+      </c>
+      <c r="B166" t="s">
         <v>314</v>
       </c>
-      <c r="B165" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="166" spans="1:2">
-      <c r="A166" t="s">
+    </row>
+    <row r="167" spans="1:3" ht="17">
+      <c r="A167" t="s">
+        <v>317</v>
+      </c>
+      <c r="B167" t="s">
         <v>316</v>
       </c>
-      <c r="B166" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="167" spans="1:2">
-      <c r="A167" t="s">
+      <c r="C167" s="3"/>
+    </row>
+    <row r="168" spans="1:3" ht="35">
+      <c r="A168" t="s">
+        <v>319</v>
+      </c>
+      <c r="B168" t="s">
         <v>318</v>
       </c>
-      <c r="B167" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="168" spans="1:2">
-      <c r="A168" t="s">
+      <c r="C168" s="2" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" ht="35">
+      <c r="A169" t="s">
         <v>320</v>
       </c>
-      <c r="B168" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="169" spans="1:2">
-      <c r="A169" t="s">
+      <c r="B169" t="s">
+        <v>288</v>
+      </c>
+      <c r="C169" s="2" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" ht="35">
+      <c r="A170" t="s">
+        <v>322</v>
+      </c>
+      <c r="B170" t="s">
         <v>321</v>
       </c>
-      <c r="B169" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="170" spans="1:2">
-      <c r="A170" t="s">
+      <c r="C170" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" ht="35">
+      <c r="A171" t="s">
+        <v>324</v>
+      </c>
+      <c r="B171" t="s">
         <v>323</v>
       </c>
-      <c r="B170" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="171" spans="1:2">
-      <c r="A171" t="s">
+      <c r="C171" s="2" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" ht="35">
+      <c r="A172">
+        <v>171</v>
+      </c>
+      <c r="B172" t="s">
         <v>325</v>
       </c>
-      <c r="B171" t="s">
-        <v>326</v>
-      </c>
+      <c r="C172" s="2" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" ht="17">
+      <c r="C173" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C171" xr:uid="{41BDCF07-C9AA-EA4C-AE1D-CCA48F6FE1DA}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>